<commit_message>
added results for large datasets
</commit_message>
<xml_diff>
--- a/results/datasheets/update-results.xlsx
+++ b/results/datasheets/update-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="old res combined" sheetId="1" r:id="rId1"/>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:S25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1621,7 +1621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371DD5AB-3C93-1647-B72B-EC6B6B0D4652}">
   <dimension ref="A1:BL433"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>

</xml_diff>